<commit_message>
last thing is to handle multiple-room bookings. the stage is set for that.
</commit_message>
<xml_diff>
--- a/invoice_items_flat_cleaned.xlsx
+++ b/invoice_items_flat_cleaned.xlsx
@@ -2946,6 +2946,9 @@
       <c r="E7">
         <v>3.5</v>
       </c>
+      <c r="F7">
+        <v>490</v>
+      </c>
       <c r="H7">
         <v>490</v>
       </c>
@@ -2964,6 +2967,9 @@
       <c r="E8">
         <v>2</v>
       </c>
+      <c r="F8">
+        <v>60</v>
+      </c>
       <c r="H8">
         <v>60</v>
       </c>
@@ -2982,6 +2988,9 @@
       <c r="E9">
         <v>1</v>
       </c>
+      <c r="F9">
+        <v>450</v>
+      </c>
       <c r="H9">
         <v>450</v>
       </c>
@@ -3000,6 +3009,9 @@
       <c r="E10">
         <v>4.5</v>
       </c>
+      <c r="F10">
+        <v>180</v>
+      </c>
       <c r="H10">
         <v>180</v>
       </c>
@@ -3220,6 +3232,9 @@
       <c r="E20">
         <v>2</v>
       </c>
+      <c r="F20">
+        <v>590</v>
+      </c>
       <c r="H20">
         <v>590</v>
       </c>
@@ -3241,6 +3256,9 @@
       <c r="E21">
         <v>2</v>
       </c>
+      <c r="F21">
+        <v>100</v>
+      </c>
       <c r="H21">
         <v>100</v>
       </c>
@@ -3262,6 +3280,9 @@
       <c r="E22">
         <v>1</v>
       </c>
+      <c r="F22">
+        <v>250</v>
+      </c>
       <c r="H22">
         <v>250</v>
       </c>
@@ -3755,6 +3776,9 @@
       <c r="E43">
         <v>6.5</v>
       </c>
+      <c r="F43">
+        <v>260</v>
+      </c>
       <c r="H43">
         <v>260</v>
       </c>
@@ -3906,6 +3930,9 @@
       <c r="E50">
         <v>2</v>
       </c>
+      <c r="F50">
+        <v>120</v>
+      </c>
       <c r="H50">
         <v>120</v>
       </c>
@@ -3927,6 +3954,9 @@
       <c r="E51">
         <v>1.5</v>
       </c>
+      <c r="F51">
+        <v>37.5</v>
+      </c>
       <c r="H51">
         <v>37.5</v>
       </c>
@@ -4457,6 +4487,9 @@
       <c r="E73">
         <v>2</v>
       </c>
+      <c r="F73">
+        <v>120</v>
+      </c>
       <c r="H73">
         <v>120</v>
       </c>
@@ -4478,6 +4511,9 @@
       <c r="E74">
         <v>1.5</v>
       </c>
+      <c r="F74">
+        <v>37.5</v>
+      </c>
       <c r="H74">
         <v>37.5</v>
       </c>
@@ -4873,6 +4909,9 @@
       <c r="E91">
         <v>4</v>
       </c>
+      <c r="F91">
+        <v>380</v>
+      </c>
       <c r="H91">
         <v>380</v>
       </c>
@@ -4891,6 +4930,9 @@
       <c r="E92">
         <v>2</v>
       </c>
+      <c r="F92">
+        <v>50</v>
+      </c>
       <c r="H92">
         <v>50</v>
       </c>
@@ -4923,6 +4965,9 @@
       <c r="E94">
         <v>4</v>
       </c>
+      <c r="F94">
+        <v>1500</v>
+      </c>
       <c r="H94">
         <v>1500</v>
       </c>
@@ -4974,6 +5019,9 @@
       <c r="E97">
         <v>4</v>
       </c>
+      <c r="F97">
+        <v>300</v>
+      </c>
       <c r="H97">
         <v>300</v>
       </c>
@@ -4995,6 +5043,9 @@
       <c r="E98">
         <v>1</v>
       </c>
+      <c r="F98">
+        <v>175</v>
+      </c>
       <c r="H98">
         <v>175</v>
       </c>
@@ -5016,6 +5067,9 @@
       <c r="E99">
         <v>1</v>
       </c>
+      <c r="F99">
+        <v>500</v>
+      </c>
       <c r="H99">
         <v>500</v>
       </c>
@@ -5037,6 +5091,9 @@
       <c r="E100">
         <v>6</v>
       </c>
+      <c r="F100">
+        <v>240</v>
+      </c>
       <c r="H100">
         <v>240</v>
       </c>
@@ -5857,6 +5914,9 @@
       <c r="E136">
         <v>1</v>
       </c>
+      <c r="F136">
+        <v>210</v>
+      </c>
       <c r="H136">
         <v>210</v>
       </c>
@@ -6011,6 +6071,9 @@
       <c r="E143">
         <v>4</v>
       </c>
+      <c r="F143">
+        <v>2000</v>
+      </c>
       <c r="H143">
         <v>2000</v>
       </c>
@@ -6092,6 +6155,9 @@
       <c r="E148">
         <v>4</v>
       </c>
+      <c r="F148">
+        <v>300</v>
+      </c>
       <c r="H148">
         <v>300</v>
       </c>
@@ -6113,6 +6179,9 @@
       <c r="E149">
         <v>1</v>
       </c>
+      <c r="F149">
+        <v>175</v>
+      </c>
       <c r="H149">
         <v>175</v>
       </c>
@@ -6134,6 +6203,9 @@
       <c r="E150">
         <v>1</v>
       </c>
+      <c r="F150">
+        <v>500</v>
+      </c>
       <c r="H150">
         <v>500</v>
       </c>
@@ -6155,6 +6227,9 @@
       <c r="E151">
         <v>5</v>
       </c>
+      <c r="F151">
+        <v>200</v>
+      </c>
       <c r="H151">
         <v>200</v>
       </c>
@@ -6390,6 +6465,9 @@
       <c r="E162">
         <v>1</v>
       </c>
+      <c r="F162">
+        <v>75</v>
+      </c>
       <c r="H162">
         <v>75</v>
       </c>
@@ -6411,6 +6489,9 @@
       <c r="E163">
         <v>3.5</v>
       </c>
+      <c r="F163">
+        <v>175</v>
+      </c>
       <c r="H163">
         <v>175</v>
       </c>
@@ -6432,6 +6513,9 @@
       <c r="E164">
         <v>1</v>
       </c>
+      <c r="F164">
+        <v>300</v>
+      </c>
       <c r="H164">
         <v>300</v>
       </c>
@@ -6453,6 +6537,9 @@
       <c r="E165">
         <v>3</v>
       </c>
+      <c r="F165">
+        <v>120</v>
+      </c>
       <c r="H165">
         <v>120</v>
       </c>
@@ -6974,6 +7061,9 @@
       <c r="E188">
         <v>2.5</v>
       </c>
+      <c r="F188">
+        <v>275</v>
+      </c>
       <c r="H188">
         <v>247.5</v>
       </c>
@@ -6992,6 +7082,9 @@
       <c r="E189">
         <v>2</v>
       </c>
+      <c r="F189">
+        <v>60</v>
+      </c>
       <c r="H189">
         <v>60</v>
       </c>
@@ -7286,6 +7379,9 @@
       <c r="E202">
         <v>2.5</v>
       </c>
+      <c r="F202">
+        <v>350</v>
+      </c>
       <c r="H202">
         <v>350</v>
       </c>
@@ -7304,6 +7400,9 @@
       <c r="E203">
         <v>2</v>
       </c>
+      <c r="F203">
+        <v>70</v>
+      </c>
       <c r="H203">
         <v>70</v>
       </c>
@@ -7378,6 +7477,9 @@
       <c r="E208">
         <v>16</v>
       </c>
+      <c r="F208">
+        <v>3280</v>
+      </c>
       <c r="G208">
         <v>0.1</v>
       </c>
@@ -7399,6 +7501,9 @@
       <c r="E209">
         <v>4</v>
       </c>
+      <c r="F209">
+        <v>100</v>
+      </c>
       <c r="H209">
         <v>100</v>
       </c>
@@ -7773,6 +7878,9 @@
       <c r="E225">
         <v>2.5</v>
       </c>
+      <c r="F225">
+        <v>562.5</v>
+      </c>
       <c r="H225">
         <v>562.5</v>
       </c>
@@ -7794,6 +7902,9 @@
       <c r="E226">
         <v>1</v>
       </c>
+      <c r="F226">
+        <v>100</v>
+      </c>
       <c r="H226">
         <v>100</v>
       </c>
@@ -8287,6 +8398,9 @@
       <c r="E248">
         <v>3</v>
       </c>
+      <c r="F248">
+        <v>825</v>
+      </c>
       <c r="H248">
         <v>825</v>
       </c>
@@ -8305,6 +8419,9 @@
       <c r="E249">
         <v>3</v>
       </c>
+      <c r="F249">
+        <v>390</v>
+      </c>
       <c r="H249">
         <v>390</v>
       </c>
@@ -8323,6 +8440,9 @@
       <c r="E250">
         <v>1</v>
       </c>
+      <c r="F250">
+        <v>500</v>
+      </c>
       <c r="H250">
         <v>500</v>
       </c>
@@ -8341,6 +8461,9 @@
       <c r="E251">
         <v>2.5</v>
       </c>
+      <c r="F251">
+        <v>62.5</v>
+      </c>
       <c r="H251">
         <v>62.5</v>
       </c>
@@ -8373,6 +8496,9 @@
       <c r="E253">
         <v>2</v>
       </c>
+      <c r="F253">
+        <v>280</v>
+      </c>
       <c r="H253">
         <v>280</v>
       </c>
@@ -8391,6 +8517,9 @@
       <c r="E254">
         <v>1</v>
       </c>
+      <c r="F254">
+        <v>50</v>
+      </c>
       <c r="H254">
         <v>50</v>
       </c>
@@ -8423,6 +8552,9 @@
       <c r="E256">
         <v>3</v>
       </c>
+      <c r="F256">
+        <v>885</v>
+      </c>
       <c r="H256">
         <v>885</v>
       </c>
@@ -8444,6 +8576,9 @@
       <c r="E257">
         <v>2</v>
       </c>
+      <c r="F257">
+        <v>100</v>
+      </c>
       <c r="H257">
         <v>100</v>
       </c>
@@ -8465,6 +8600,9 @@
       <c r="E258">
         <v>1</v>
       </c>
+      <c r="F258">
+        <v>250</v>
+      </c>
       <c r="H258">
         <v>250</v>
       </c>
@@ -8574,6 +8712,9 @@
       <c r="E263">
         <v>2.5</v>
       </c>
+      <c r="F263">
+        <v>275</v>
+      </c>
       <c r="H263">
         <v>275</v>
       </c>
@@ -8592,6 +8733,9 @@
       <c r="E264">
         <v>1.5</v>
       </c>
+      <c r="F264">
+        <v>52.5</v>
+      </c>
       <c r="H264">
         <v>52.5</v>
       </c>
@@ -8785,6 +8929,9 @@
       <c r="E274">
         <v>1</v>
       </c>
+      <c r="F274">
+        <v>30</v>
+      </c>
       <c r="H274">
         <v>30</v>
       </c>
@@ -9258,6 +9405,9 @@
       <c r="E294">
         <v>1</v>
       </c>
+      <c r="F294">
+        <v>749</v>
+      </c>
       <c r="H294">
         <v>749</v>
       </c>
@@ -9279,6 +9429,9 @@
       <c r="E295">
         <v>1</v>
       </c>
+      <c r="F295">
+        <v>140</v>
+      </c>
       <c r="H295">
         <v>140</v>
       </c>
@@ -9300,6 +9453,9 @@
       <c r="E296">
         <v>2.5</v>
       </c>
+      <c r="F296">
+        <v>100</v>
+      </c>
       <c r="H296">
         <v>100</v>
       </c>
@@ -9321,6 +9477,9 @@
       <c r="E297">
         <v>1</v>
       </c>
+      <c r="F297">
+        <v>757</v>
+      </c>
       <c r="H297">
         <v>757</v>
       </c>
@@ -9342,6 +9501,9 @@
       <c r="E298">
         <v>17</v>
       </c>
+      <c r="F298">
+        <v>850</v>
+      </c>
       <c r="H298">
         <v>850</v>
       </c>
@@ -9618,6 +9780,9 @@
       <c r="E310">
         <v>1</v>
       </c>
+      <c r="F310">
+        <v>75</v>
+      </c>
       <c r="H310">
         <v>0</v>
       </c>
@@ -9663,6 +9828,9 @@
       <c r="E312">
         <v>1</v>
       </c>
+      <c r="F312">
+        <v>500</v>
+      </c>
       <c r="H312">
         <v>0</v>
       </c>
@@ -9749,6 +9917,9 @@
       <c r="E316">
         <v>20</v>
       </c>
+      <c r="F316">
+        <v>4000</v>
+      </c>
       <c r="H316">
         <v>4000</v>
       </c>
@@ -9770,6 +9941,9 @@
       <c r="E317">
         <v>7</v>
       </c>
+      <c r="F317">
+        <v>350</v>
+      </c>
       <c r="H317">
         <v>350</v>
       </c>
@@ -9791,6 +9965,9 @@
       <c r="E318">
         <v>1</v>
       </c>
+      <c r="F318">
+        <v>650</v>
+      </c>
       <c r="H318">
         <v>650</v>
       </c>
@@ -9812,6 +9989,9 @@
       <c r="E319">
         <v>7</v>
       </c>
+      <c r="F319">
+        <v>280</v>
+      </c>
       <c r="H319">
         <v>280</v>
       </c>
@@ -10310,7 +10490,7 @@
         <v>4</v>
       </c>
       <c r="F340">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="G340">
         <v>1</v>
@@ -11303,6 +11483,9 @@
       <c r="E382">
         <v>3</v>
       </c>
+      <c r="F382">
+        <v>420</v>
+      </c>
       <c r="H382">
         <v>420</v>
       </c>
@@ -11324,6 +11507,9 @@
       <c r="E383">
         <v>2</v>
       </c>
+      <c r="F383">
+        <v>100</v>
+      </c>
       <c r="H383">
         <v>100</v>
       </c>
@@ -11345,6 +11531,9 @@
       <c r="E384">
         <v>1</v>
       </c>
+      <c r="F384">
+        <v>250</v>
+      </c>
       <c r="H384">
         <v>250</v>
       </c>
@@ -11366,6 +11555,9 @@
       <c r="E385">
         <v>2</v>
       </c>
+      <c r="F385">
+        <v>80</v>
+      </c>
       <c r="H385">
         <v>80</v>
       </c>
@@ -12035,6 +12227,9 @@
       <c r="E414">
         <v>6</v>
       </c>
+      <c r="F414">
+        <v>240</v>
+      </c>
       <c r="H414">
         <v>240</v>
       </c>
@@ -12067,6 +12262,9 @@
       <c r="E416">
         <v>2</v>
       </c>
+      <c r="F416">
+        <v>590</v>
+      </c>
       <c r="H416">
         <v>590</v>
       </c>
@@ -12088,6 +12286,9 @@
       <c r="E417">
         <v>3.5</v>
       </c>
+      <c r="F417">
+        <v>175</v>
+      </c>
       <c r="H417">
         <v>175</v>
       </c>
@@ -12109,6 +12310,9 @@
       <c r="E418">
         <v>1</v>
       </c>
+      <c r="F418">
+        <v>250</v>
+      </c>
       <c r="H418">
         <v>250</v>
       </c>
@@ -12130,6 +12334,9 @@
       <c r="E419">
         <v>2</v>
       </c>
+      <c r="F419">
+        <v>80</v>
+      </c>
       <c r="H419">
         <v>80</v>
       </c>
@@ -12364,6 +12571,9 @@
       <c r="E430">
         <v>2</v>
       </c>
+      <c r="F430">
+        <v>0</v>
+      </c>
       <c r="H430">
         <v>0</v>
       </c>
@@ -12382,6 +12592,9 @@
       <c r="E431">
         <v>2</v>
       </c>
+      <c r="F431">
+        <v>0</v>
+      </c>
       <c r="H431">
         <v>0</v>
       </c>
@@ -12415,6 +12628,9 @@
       <c r="E433">
         <v>3.5</v>
       </c>
+      <c r="F433">
+        <v>105</v>
+      </c>
       <c r="H433">
         <v>105</v>
       </c>
@@ -12498,6 +12714,9 @@
       <c r="E437">
         <v>1</v>
       </c>
+      <c r="F437">
+        <v>250</v>
+      </c>
       <c r="H437">
         <v>0</v>
       </c>
@@ -12563,6 +12782,9 @@
       <c r="E440">
         <v>2</v>
       </c>
+      <c r="F440">
+        <v>300</v>
+      </c>
       <c r="H440">
         <v>300</v>
       </c>
@@ -12581,6 +12803,9 @@
       <c r="E441">
         <v>2</v>
       </c>
+      <c r="F441">
+        <v>100</v>
+      </c>
       <c r="H441">
         <v>100</v>
       </c>
@@ -12599,6 +12824,9 @@
       <c r="E442">
         <v>1</v>
       </c>
+      <c r="F442">
+        <v>100</v>
+      </c>
       <c r="H442">
         <v>100</v>
       </c>
@@ -12631,6 +12859,9 @@
       <c r="E444">
         <v>1</v>
       </c>
+      <c r="F444">
+        <v>100</v>
+      </c>
       <c r="H444">
         <v>100</v>
       </c>
@@ -12663,6 +12894,9 @@
       <c r="E446">
         <v>3</v>
       </c>
+      <c r="F446">
+        <v>186</v>
+      </c>
       <c r="H446">
         <v>186</v>
       </c>
@@ -12684,6 +12918,9 @@
       <c r="E447">
         <v>2.5</v>
       </c>
+      <c r="F447">
+        <v>125</v>
+      </c>
       <c r="H447">
         <v>125</v>
       </c>
@@ -12705,6 +12942,9 @@
       <c r="E448">
         <v>1</v>
       </c>
+      <c r="F448">
+        <v>250</v>
+      </c>
       <c r="H448">
         <v>250</v>
       </c>
@@ -12726,6 +12966,9 @@
       <c r="E449">
         <v>4</v>
       </c>
+      <c r="F449">
+        <v>160</v>
+      </c>
       <c r="H449">
         <v>160</v>
       </c>
@@ -12747,6 +12990,9 @@
       <c r="E450">
         <v>1</v>
       </c>
+      <c r="F450">
+        <v>29</v>
+      </c>
       <c r="H450">
         <v>29</v>
       </c>
@@ -12877,6 +13123,9 @@
       <c r="E456">
         <v>1</v>
       </c>
+      <c r="F456">
+        <v>250</v>
+      </c>
       <c r="H456">
         <v>250</v>
       </c>
@@ -12909,6 +13158,9 @@
       <c r="E458">
         <v>5</v>
       </c>
+      <c r="F458">
+        <v>425</v>
+      </c>
       <c r="H458">
         <v>425</v>
       </c>
@@ -12930,6 +13182,9 @@
       <c r="E459">
         <v>5</v>
       </c>
+      <c r="F459">
+        <v>650</v>
+      </c>
       <c r="H459">
         <v>650</v>
       </c>
@@ -12951,6 +13206,9 @@
       <c r="E460">
         <v>5</v>
       </c>
+      <c r="F460">
+        <v>1025</v>
+      </c>
       <c r="H460">
         <v>1025</v>
       </c>
@@ -12972,6 +13230,9 @@
       <c r="E461">
         <v>5</v>
       </c>
+      <c r="F461">
+        <v>925</v>
+      </c>
       <c r="H461">
         <v>925</v>
       </c>
@@ -12993,6 +13254,9 @@
       <c r="E462">
         <v>6</v>
       </c>
+      <c r="F462">
+        <v>240</v>
+      </c>
       <c r="H462">
         <v>240</v>
       </c>
@@ -13014,6 +13278,9 @@
       <c r="E463">
         <v>5</v>
       </c>
+      <c r="F463">
+        <v>250</v>
+      </c>
       <c r="H463">
         <v>250</v>
       </c>
@@ -13749,6 +14016,9 @@
       <c r="E494">
         <v>1</v>
       </c>
+      <c r="F494">
+        <v>50</v>
+      </c>
       <c r="H494">
         <v>50</v>
       </c>
@@ -13781,6 +14051,9 @@
       <c r="E496">
         <v>2</v>
       </c>
+      <c r="F496">
+        <v>450</v>
+      </c>
       <c r="H496">
         <v>450</v>
       </c>
@@ -13802,6 +14075,9 @@
       <c r="E497">
         <v>2.5</v>
       </c>
+      <c r="F497">
+        <v>125</v>
+      </c>
       <c r="H497">
         <v>125</v>
       </c>
@@ -13823,6 +14099,9 @@
       <c r="E498">
         <v>1</v>
       </c>
+      <c r="F498">
+        <v>250</v>
+      </c>
       <c r="H498">
         <v>250</v>
       </c>
@@ -13952,6 +14231,9 @@
       <c r="E504">
         <v>3</v>
       </c>
+      <c r="F504">
+        <v>420</v>
+      </c>
       <c r="H504">
         <v>420</v>
       </c>
@@ -13973,6 +14255,9 @@
       <c r="E505">
         <v>2</v>
       </c>
+      <c r="F505">
+        <v>100</v>
+      </c>
       <c r="H505">
         <v>100</v>
       </c>
@@ -13994,6 +14279,9 @@
       <c r="E506">
         <v>1</v>
       </c>
+      <c r="F506">
+        <v>250</v>
+      </c>
       <c r="H506">
         <v>250</v>
       </c>
@@ -14479,6 +14767,9 @@
       <c r="E526">
         <v>3</v>
       </c>
+      <c r="F526">
+        <v>180</v>
+      </c>
       <c r="H526">
         <v>180</v>
       </c>
@@ -15100,6 +15391,9 @@
       <c r="E553">
         <v>3.5</v>
       </c>
+      <c r="F553">
+        <v>1032.5</v>
+      </c>
       <c r="H553">
         <v>1032.5</v>
       </c>
@@ -15121,6 +15415,9 @@
       <c r="E554">
         <v>3.5</v>
       </c>
+      <c r="F554">
+        <v>682.5</v>
+      </c>
       <c r="H554">
         <v>682.5</v>
       </c>
@@ -15142,6 +15439,9 @@
       <c r="E555">
         <v>2.5</v>
       </c>
+      <c r="F555">
+        <v>125</v>
+      </c>
       <c r="H555">
         <v>125</v>
       </c>
@@ -15163,6 +15463,9 @@
       <c r="E556">
         <v>1</v>
       </c>
+      <c r="F556">
+        <v>500</v>
+      </c>
       <c r="H556">
         <v>500</v>
       </c>
@@ -15184,6 +15487,9 @@
       <c r="E557">
         <v>2</v>
       </c>
+      <c r="F557">
+        <v>60</v>
+      </c>
       <c r="H557">
         <v>60</v>
       </c>
@@ -15417,6 +15723,9 @@
       <c r="E570">
         <v>2.5</v>
       </c>
+      <c r="F570">
+        <v>250</v>
+      </c>
       <c r="H570">
         <v>250</v>
       </c>
@@ -15438,6 +15747,9 @@
       <c r="E571">
         <v>1</v>
       </c>
+      <c r="F571">
+        <v>50</v>
+      </c>
       <c r="H571">
         <v>50</v>
       </c>
@@ -16764,6 +17076,9 @@
       <c r="E628">
         <v>3</v>
       </c>
+      <c r="F628">
+        <v>825</v>
+      </c>
       <c r="H628">
         <v>825</v>
       </c>
@@ -16782,6 +17097,9 @@
       <c r="E629">
         <v>3</v>
       </c>
+      <c r="F629">
+        <v>390</v>
+      </c>
       <c r="H629">
         <v>390</v>
       </c>
@@ -16800,6 +17118,9 @@
       <c r="E630">
         <v>1</v>
       </c>
+      <c r="F630">
+        <v>500</v>
+      </c>
       <c r="H630">
         <v>500</v>
       </c>
@@ -16818,6 +17139,9 @@
       <c r="E631">
         <v>4.5</v>
       </c>
+      <c r="F631">
+        <v>67.5</v>
+      </c>
       <c r="H631">
         <v>67.5</v>
       </c>
@@ -17027,7 +17351,7 @@
         <v>4.5</v>
       </c>
       <c r="F640">
-        <v>350</v>
+        <v>180</v>
       </c>
       <c r="H640">
         <v>350</v>
@@ -17238,6 +17562,9 @@
       <c r="E650">
         <v>2</v>
       </c>
+      <c r="F650">
+        <v>280</v>
+      </c>
       <c r="H650">
         <v>280</v>
       </c>
@@ -17256,6 +17583,9 @@
       <c r="E651">
         <v>1</v>
       </c>
+      <c r="F651">
+        <v>50</v>
+      </c>
       <c r="H651">
         <v>50</v>
       </c>
@@ -17288,6 +17618,9 @@
       <c r="E653">
         <v>4</v>
       </c>
+      <c r="F653">
+        <v>560</v>
+      </c>
       <c r="H653">
         <v>560</v>
       </c>
@@ -17309,6 +17642,9 @@
       <c r="E654">
         <v>2</v>
       </c>
+      <c r="F654">
+        <v>100</v>
+      </c>
       <c r="H654">
         <v>100</v>
       </c>
@@ -17330,6 +17666,9 @@
       <c r="E655">
         <v>1</v>
       </c>
+      <c r="F655">
+        <v>250</v>
+      </c>
       <c r="H655">
         <v>250</v>
       </c>
@@ -17351,6 +17690,9 @@
       <c r="E656">
         <v>2</v>
       </c>
+      <c r="F656">
+        <v>80</v>
+      </c>
       <c r="H656">
         <v>80</v>
       </c>
@@ -17824,6 +18166,9 @@
       <c r="E677">
         <v>2.5</v>
       </c>
+      <c r="F677">
+        <v>225</v>
+      </c>
       <c r="H677">
         <v>225</v>
       </c>
@@ -17842,6 +18187,9 @@
       <c r="E678">
         <v>2</v>
       </c>
+      <c r="F678">
+        <v>50</v>
+      </c>
       <c r="H678">
         <v>50</v>
       </c>
@@ -17874,6 +18222,9 @@
       <c r="E680">
         <v>5</v>
       </c>
+      <c r="F680">
+        <v>200</v>
+      </c>
       <c r="H680">
         <v>200</v>
       </c>
@@ -17912,6 +18263,9 @@
       <c r="E682">
         <v>3</v>
       </c>
+      <c r="F682">
+        <v>330</v>
+      </c>
       <c r="H682">
         <v>297</v>
       </c>
@@ -17930,6 +18284,9 @@
       <c r="E683">
         <v>2</v>
       </c>
+      <c r="F683">
+        <v>60</v>
+      </c>
       <c r="H683">
         <v>60</v>
       </c>
@@ -17948,6 +18305,9 @@
       <c r="E684">
         <v>1</v>
       </c>
+      <c r="F684">
+        <v>150</v>
+      </c>
       <c r="H684">
         <v>150</v>
       </c>
@@ -18024,6 +18384,9 @@
       <c r="E688">
         <v>1</v>
       </c>
+      <c r="F688">
+        <v>50</v>
+      </c>
       <c r="H688">
         <v>50</v>
       </c>
@@ -18613,6 +18976,9 @@
       <c r="E714">
         <v>1</v>
       </c>
+      <c r="F714">
+        <v>75</v>
+      </c>
       <c r="H714">
         <v>0</v>
       </c>
@@ -18658,6 +19024,9 @@
       <c r="E716">
         <v>1</v>
       </c>
+      <c r="F716">
+        <v>500</v>
+      </c>
       <c r="H716">
         <v>0</v>
       </c>
@@ -18816,7 +19185,7 @@
         <v>2.5</v>
       </c>
       <c r="F723">
-        <v>115</v>
+        <v>287.5</v>
       </c>
       <c r="H723">
         <v>115</v>
@@ -18931,6 +19300,9 @@
       <c r="E728">
         <v>5.5</v>
       </c>
+      <c r="F728">
+        <v>1402.5</v>
+      </c>
       <c r="H728">
         <v>1402.5</v>
       </c>
@@ -18952,6 +19324,9 @@
       <c r="E729">
         <v>1.5</v>
       </c>
+      <c r="F729">
+        <v>75</v>
+      </c>
       <c r="H729">
         <v>75</v>
       </c>
@@ -18973,6 +19348,9 @@
       <c r="E730">
         <v>1</v>
       </c>
+      <c r="F730">
+        <v>250</v>
+      </c>
       <c r="H730">
         <v>250</v>
       </c>
@@ -19279,6 +19657,9 @@
       <c r="E743">
         <v>4</v>
       </c>
+      <c r="F743">
+        <v>1100</v>
+      </c>
       <c r="H743">
         <v>1100</v>
       </c>
@@ -19891,6 +20272,9 @@
       <c r="E770">
         <v>4</v>
       </c>
+      <c r="F770">
+        <v>200</v>
+      </c>
       <c r="H770">
         <v>200</v>
       </c>
@@ -19933,6 +20317,9 @@
       <c r="E772">
         <v>1</v>
       </c>
+      <c r="F772">
+        <v>50</v>
+      </c>
       <c r="H772">
         <v>50</v>
       </c>
@@ -20313,6 +20700,9 @@
       <c r="E789">
         <v>3</v>
       </c>
+      <c r="F789">
+        <v>270</v>
+      </c>
       <c r="H789">
         <v>270</v>
       </c>
@@ -20334,6 +20724,9 @@
       <c r="E790">
         <v>1</v>
       </c>
+      <c r="F790">
+        <v>50</v>
+      </c>
       <c r="H790">
         <v>50</v>
       </c>
@@ -20548,6 +20941,9 @@
       <c r="E799">
         <v>2.5</v>
       </c>
+      <c r="F799">
+        <v>350</v>
+      </c>
       <c r="H799">
         <v>350</v>
       </c>
@@ -20614,6 +21010,9 @@
       <c r="E802">
         <v>4</v>
       </c>
+      <c r="F802">
+        <v>160</v>
+      </c>
       <c r="H802">
         <v>160</v>
       </c>
@@ -20646,6 +21045,9 @@
       <c r="E804">
         <v>2</v>
       </c>
+      <c r="F804">
+        <v>300</v>
+      </c>
       <c r="H804">
         <v>300</v>
       </c>
@@ -20664,6 +21066,9 @@
       <c r="E805">
         <v>2</v>
       </c>
+      <c r="F805">
+        <v>100</v>
+      </c>
       <c r="H805">
         <v>100</v>
       </c>
@@ -20682,6 +21087,9 @@
       <c r="E806">
         <v>1</v>
       </c>
+      <c r="F806">
+        <v>100</v>
+      </c>
       <c r="H806">
         <v>100</v>
       </c>
@@ -21071,6 +21479,9 @@
       <c r="E823">
         <v>5</v>
       </c>
+      <c r="F823">
+        <v>625</v>
+      </c>
       <c r="H823">
         <v>625</v>
       </c>
@@ -21092,6 +21503,9 @@
       <c r="E824">
         <v>2</v>
       </c>
+      <c r="F824">
+        <v>60</v>
+      </c>
       <c r="H824">
         <v>60</v>
       </c>
@@ -21130,6 +21544,9 @@
       <c r="E826">
         <v>2.5</v>
       </c>
+      <c r="F826">
+        <v>350</v>
+      </c>
       <c r="H826">
         <v>350</v>
       </c>
@@ -21148,6 +21565,9 @@
       <c r="E827">
         <v>2</v>
       </c>
+      <c r="F827">
+        <v>70</v>
+      </c>
       <c r="H827">
         <v>70</v>
       </c>
@@ -21541,6 +21961,9 @@
       <c r="E845">
         <v>7</v>
       </c>
+      <c r="F845">
+        <v>980</v>
+      </c>
       <c r="H845">
         <v>980</v>
       </c>
@@ -21559,6 +21982,9 @@
       <c r="E846">
         <v>4</v>
       </c>
+      <c r="F846">
+        <v>240</v>
+      </c>
       <c r="H846">
         <v>240</v>
       </c>
@@ -21577,6 +22003,9 @@
       <c r="E847">
         <v>4</v>
       </c>
+      <c r="F847">
+        <v>360</v>
+      </c>
       <c r="H847">
         <v>360</v>
       </c>
@@ -21595,6 +22024,9 @@
       <c r="E848">
         <v>4</v>
       </c>
+      <c r="F848">
+        <v>100</v>
+      </c>
       <c r="H848">
         <v>100</v>
       </c>
@@ -21613,6 +22045,9 @@
       <c r="E849">
         <v>3</v>
       </c>
+      <c r="F849">
+        <v>150</v>
+      </c>
       <c r="H849">
         <v>150</v>
       </c>
@@ -21645,6 +22080,9 @@
       <c r="E851">
         <v>7.5</v>
       </c>
+      <c r="F851">
+        <v>637.5</v>
+      </c>
       <c r="G851">
         <v>0.1</v>
       </c>
@@ -21666,6 +22104,9 @@
       <c r="E852">
         <v>15</v>
       </c>
+      <c r="F852">
+        <v>3075</v>
+      </c>
       <c r="G852">
         <v>0.1</v>
       </c>
@@ -21687,6 +22128,9 @@
       <c r="E853">
         <v>15</v>
       </c>
+      <c r="F853">
+        <v>0</v>
+      </c>
       <c r="H853">
         <v>0</v>
       </c>
@@ -21705,6 +22149,9 @@
       <c r="E854">
         <v>15</v>
       </c>
+      <c r="F854">
+        <v>0</v>
+      </c>
       <c r="H854">
         <v>0</v>
       </c>
@@ -21723,6 +22170,9 @@
       <c r="E855">
         <v>3</v>
       </c>
+      <c r="F855">
+        <v>150</v>
+      </c>
       <c r="H855">
         <v>150</v>
       </c>
@@ -22305,6 +22755,9 @@
       <c r="E881">
         <v>4</v>
       </c>
+      <c r="F881">
+        <v>1180</v>
+      </c>
       <c r="H881">
         <v>1180</v>
       </c>
@@ -22323,6 +22776,9 @@
       <c r="E882">
         <v>3</v>
       </c>
+      <c r="F882">
+        <v>105</v>
+      </c>
       <c r="H882">
         <v>105</v>
       </c>
@@ -22778,6 +23234,9 @@
       <c r="E903">
         <v>2.5</v>
       </c>
+      <c r="F903">
+        <v>275</v>
+      </c>
       <c r="H903">
         <v>275</v>
       </c>
@@ -22796,6 +23255,9 @@
       <c r="E904">
         <v>1.5</v>
       </c>
+      <c r="F904">
+        <v>52.5</v>
+      </c>
       <c r="H904">
         <v>52.5</v>
       </c>
@@ -22870,6 +23332,9 @@
       <c r="E909">
         <v>4</v>
       </c>
+      <c r="F909">
+        <v>560</v>
+      </c>
       <c r="H909">
         <v>560</v>
       </c>
@@ -22891,6 +23356,9 @@
       <c r="E910">
         <v>4</v>
       </c>
+      <c r="F910">
+        <v>220</v>
+      </c>
       <c r="H910">
         <v>220</v>
       </c>
@@ -22912,6 +23380,9 @@
       <c r="E911">
         <v>0</v>
       </c>
+      <c r="F911">
+        <v>0</v>
+      </c>
       <c r="H911">
         <v>0</v>
       </c>
@@ -23887,6 +24358,9 @@
       <c r="E953">
         <v>6</v>
       </c>
+      <c r="F953">
+        <v>510</v>
+      </c>
       <c r="H953">
         <v>510</v>
       </c>
@@ -23905,6 +24379,9 @@
       <c r="E954">
         <v>6</v>
       </c>
+      <c r="F954">
+        <v>780</v>
+      </c>
       <c r="H954">
         <v>780</v>
       </c>
@@ -23923,6 +24400,9 @@
       <c r="E955">
         <v>6</v>
       </c>
+      <c r="F955">
+        <v>1230</v>
+      </c>
       <c r="H955">
         <v>1230</v>
       </c>
@@ -23941,6 +24421,9 @@
       <c r="E956">
         <v>6</v>
       </c>
+      <c r="F956">
+        <v>690</v>
+      </c>
       <c r="H956">
         <v>690</v>
       </c>
@@ -23959,6 +24442,9 @@
       <c r="E957">
         <v>6</v>
       </c>
+      <c r="F957">
+        <v>240</v>
+      </c>
       <c r="H957">
         <v>240</v>
       </c>
@@ -23977,6 +24463,9 @@
       <c r="E958">
         <v>4</v>
       </c>
+      <c r="F958">
+        <v>200</v>
+      </c>
       <c r="H958">
         <v>200</v>
       </c>
@@ -24024,6 +24513,9 @@
       <c r="E961">
         <v>2</v>
       </c>
+      <c r="F961">
+        <v>590</v>
+      </c>
       <c r="H961">
         <v>590</v>
       </c>
@@ -24045,6 +24537,9 @@
       <c r="E962">
         <v>2.5</v>
       </c>
+      <c r="F962">
+        <v>125</v>
+      </c>
       <c r="H962">
         <v>125</v>
       </c>
@@ -24066,6 +24561,9 @@
       <c r="E963">
         <v>1</v>
       </c>
+      <c r="F963">
+        <v>250</v>
+      </c>
       <c r="H963">
         <v>250</v>
       </c>
@@ -24087,6 +24585,9 @@
       <c r="E964">
         <v>1</v>
       </c>
+      <c r="F964">
+        <v>40</v>
+      </c>
       <c r="H964">
         <v>40</v>
       </c>
@@ -24244,6 +24745,9 @@
       <c r="E971">
         <v>4</v>
       </c>
+      <c r="F971">
+        <v>820</v>
+      </c>
       <c r="H971">
         <v>820</v>
       </c>
@@ -24265,6 +24769,9 @@
       <c r="E972">
         <v>4</v>
       </c>
+      <c r="F972">
+        <v>600</v>
+      </c>
       <c r="H972">
         <v>600</v>
       </c>
@@ -24286,6 +24793,9 @@
       <c r="E973">
         <v>4</v>
       </c>
+      <c r="F973">
+        <v>200</v>
+      </c>
       <c r="H973">
         <v>200</v>
       </c>
@@ -24307,6 +24817,9 @@
       <c r="E974">
         <v>1</v>
       </c>
+      <c r="F974">
+        <v>250</v>
+      </c>
       <c r="H974">
         <v>250</v>
       </c>
@@ -25152,7 +25665,7 @@
         <v>1</v>
       </c>
       <c r="F1011">
-        <v>44</v>
+        <v>44.33</v>
       </c>
       <c r="H1011">
         <v>44</v>
@@ -25195,6 +25708,9 @@
       <c r="E1013">
         <v>3</v>
       </c>
+      <c r="F1013">
+        <v>825</v>
+      </c>
       <c r="H1013">
         <v>825</v>
       </c>
@@ -25228,6 +25744,9 @@
       <c r="E1015">
         <v>2</v>
       </c>
+      <c r="F1015">
+        <v>50</v>
+      </c>
       <c r="H1015">
         <v>50</v>
       </c>
@@ -25575,6 +26094,9 @@
       <c r="E1031">
         <v>3</v>
       </c>
+      <c r="F1031">
+        <v>675</v>
+      </c>
       <c r="H1031">
         <v>675</v>
       </c>
@@ -25596,6 +26118,9 @@
       <c r="E1032">
         <v>3</v>
       </c>
+      <c r="F1032">
+        <v>450</v>
+      </c>
       <c r="H1032">
         <v>450</v>
       </c>
@@ -25617,6 +26142,9 @@
       <c r="E1033">
         <v>3.5</v>
       </c>
+      <c r="F1033">
+        <v>175</v>
+      </c>
       <c r="H1033">
         <v>175</v>
       </c>
@@ -25638,6 +26166,9 @@
       <c r="E1034">
         <v>1</v>
       </c>
+      <c r="F1034">
+        <v>350</v>
+      </c>
       <c r="H1034">
         <v>350</v>
       </c>
@@ -25659,6 +26190,9 @@
       <c r="E1035">
         <v>5</v>
       </c>
+      <c r="F1035">
+        <v>200</v>
+      </c>
       <c r="H1035">
         <v>200</v>
       </c>
@@ -25680,6 +26214,9 @@
       <c r="E1036">
         <v>1</v>
       </c>
+      <c r="F1036">
+        <v>75</v>
+      </c>
       <c r="H1036">
         <v>75</v>
       </c>
@@ -25701,6 +26238,9 @@
       <c r="E1037">
         <v>1</v>
       </c>
+      <c r="F1037">
+        <v>30</v>
+      </c>
       <c r="H1037">
         <v>30</v>
       </c>
@@ -26430,6 +26970,9 @@
       <c r="E1068">
         <v>2.5</v>
       </c>
+      <c r="F1068">
+        <v>437.5</v>
+      </c>
       <c r="H1068">
         <v>393.75</v>
       </c>
@@ -26448,6 +26991,9 @@
       <c r="E1069">
         <v>2</v>
       </c>
+      <c r="F1069">
+        <v>60</v>
+      </c>
       <c r="H1069">
         <v>60</v>
       </c>
@@ -27355,6 +27901,9 @@
       <c r="E1109">
         <v>3</v>
       </c>
+      <c r="F1109">
+        <v>420</v>
+      </c>
       <c r="H1109">
         <v>420</v>
       </c>
@@ -27373,6 +27922,9 @@
       <c r="E1110">
         <v>2</v>
       </c>
+      <c r="F1110">
+        <v>70</v>
+      </c>
       <c r="H1110">
         <v>70</v>
       </c>
@@ -28167,6 +28719,9 @@
       <c r="E1146">
         <v>4</v>
       </c>
+      <c r="F1146">
+        <v>900</v>
+      </c>
       <c r="H1146">
         <v>900</v>
       </c>
@@ -28188,6 +28743,9 @@
       <c r="E1147">
         <v>4</v>
       </c>
+      <c r="F1147">
+        <v>600</v>
+      </c>
       <c r="H1147">
         <v>600</v>
       </c>
@@ -28209,6 +28767,9 @@
       <c r="E1148">
         <v>3.5</v>
       </c>
+      <c r="F1148">
+        <v>175</v>
+      </c>
       <c r="H1148">
         <v>175</v>
       </c>
@@ -28230,6 +28791,9 @@
       <c r="E1149">
         <v>1</v>
       </c>
+      <c r="F1149">
+        <v>500</v>
+      </c>
       <c r="H1149">
         <v>500</v>
       </c>
@@ -28680,6 +29244,9 @@
       <c r="E1168">
         <v>2</v>
       </c>
+      <c r="F1168">
+        <v>120</v>
+      </c>
       <c r="H1168">
         <v>120</v>
       </c>
@@ -28701,6 +29268,9 @@
       <c r="E1169">
         <v>1.5</v>
       </c>
+      <c r="F1169">
+        <v>37.5</v>
+      </c>
       <c r="H1169">
         <v>37.5</v>
       </c>
@@ -29147,6 +29717,9 @@
       <c r="E1188">
         <v>2</v>
       </c>
+      <c r="F1188">
+        <v>80</v>
+      </c>
       <c r="H1188">
         <v>560</v>
       </c>
@@ -30012,6 +30585,9 @@
       <c r="E1227">
         <v>2.5</v>
       </c>
+      <c r="F1227">
+        <v>737.5</v>
+      </c>
       <c r="H1227">
         <v>737.5</v>
       </c>
@@ -30033,6 +30609,9 @@
       <c r="E1228">
         <v>1.75</v>
       </c>
+      <c r="F1228">
+        <v>87.5</v>
+      </c>
       <c r="H1228">
         <v>87.5</v>
       </c>
@@ -30054,6 +30633,9 @@
       <c r="E1229">
         <v>1</v>
       </c>
+      <c r="F1229">
+        <v>250</v>
+      </c>
       <c r="H1229">
         <v>250</v>
       </c>
@@ -30075,6 +30657,9 @@
       <c r="E1230">
         <v>1</v>
       </c>
+      <c r="F1230">
+        <v>100</v>
+      </c>
       <c r="H1230">
         <v>100</v>
       </c>
@@ -30096,6 +30681,9 @@
       <c r="E1231">
         <v>4.25</v>
       </c>
+      <c r="F1231">
+        <v>170</v>
+      </c>
       <c r="H1231">
         <v>170</v>
       </c>
@@ -30253,6 +30841,9 @@
       <c r="E1238">
         <v>3</v>
       </c>
+      <c r="F1238">
+        <v>420</v>
+      </c>
       <c r="H1238">
         <v>420</v>
       </c>
@@ -30274,6 +30865,9 @@
       <c r="E1239">
         <v>2</v>
       </c>
+      <c r="F1239">
+        <v>100</v>
+      </c>
       <c r="H1239">
         <v>100</v>
       </c>
@@ -30295,6 +30889,9 @@
       <c r="E1240">
         <v>1</v>
       </c>
+      <c r="F1240">
+        <v>250</v>
+      </c>
       <c r="H1240">
         <v>250</v>
       </c>
@@ -30960,6 +31557,9 @@
       <c r="E1269">
         <v>5.5</v>
       </c>
+      <c r="F1269">
+        <v>1402.5</v>
+      </c>
       <c r="H1269">
         <v>1402.5</v>
       </c>
@@ -30981,6 +31581,9 @@
       <c r="E1270">
         <v>5.5</v>
       </c>
+      <c r="F1270">
+        <v>825</v>
+      </c>
       <c r="H1270">
         <v>825</v>
       </c>
@@ -31002,6 +31605,9 @@
       <c r="E1271">
         <v>1</v>
       </c>
+      <c r="F1271">
+        <v>250</v>
+      </c>
       <c r="H1271">
         <v>250</v>
       </c>
@@ -31023,6 +31629,9 @@
       <c r="E1272">
         <v>2</v>
       </c>
+      <c r="F1272">
+        <v>100</v>
+      </c>
       <c r="H1272">
         <v>100</v>
       </c>
@@ -31180,6 +31789,9 @@
       <c r="E1279">
         <v>5</v>
       </c>
+      <c r="F1279">
+        <v>900</v>
+      </c>
       <c r="H1279">
         <v>900</v>
       </c>
@@ -31201,6 +31813,9 @@
       <c r="E1280">
         <v>5</v>
       </c>
+      <c r="F1280">
+        <v>150</v>
+      </c>
       <c r="H1280">
         <v>150</v>
       </c>
@@ -31222,6 +31837,9 @@
       <c r="E1281">
         <v>1</v>
       </c>
+      <c r="F1281">
+        <v>500</v>
+      </c>
       <c r="H1281">
         <v>500</v>
       </c>
@@ -31243,6 +31861,9 @@
       <c r="E1282">
         <v>6.5</v>
       </c>
+      <c r="F1282">
+        <v>260</v>
+      </c>
       <c r="H1282">
         <v>260</v>
       </c>
@@ -31561,6 +32182,9 @@
       <c r="E1296">
         <v>2</v>
       </c>
+      <c r="F1296">
+        <v>300</v>
+      </c>
       <c r="H1296">
         <v>300</v>
       </c>
@@ -31579,6 +32203,9 @@
       <c r="E1297">
         <v>2</v>
       </c>
+      <c r="F1297">
+        <v>100</v>
+      </c>
       <c r="H1297">
         <v>100</v>
       </c>
@@ -31597,6 +32224,9 @@
       <c r="E1298">
         <v>1</v>
       </c>
+      <c r="F1298">
+        <v>100</v>
+      </c>
       <c r="H1298">
         <v>100</v>
       </c>
@@ -32790,6 +33420,9 @@
       <c r="E1348">
         <v>2.5</v>
       </c>
+      <c r="F1348">
+        <v>562.5</v>
+      </c>
       <c r="H1348">
         <v>562.5</v>
       </c>
@@ -32811,6 +33444,9 @@
       <c r="E1349">
         <v>2</v>
       </c>
+      <c r="F1349">
+        <v>100</v>
+      </c>
       <c r="H1349">
         <v>100</v>
       </c>
@@ -32832,6 +33468,9 @@
       <c r="E1350">
         <v>1</v>
       </c>
+      <c r="F1350">
+        <v>250</v>
+      </c>
       <c r="H1350">
         <v>250</v>
       </c>
@@ -33275,6 +33914,9 @@
       <c r="E1369">
         <v>1</v>
       </c>
+      <c r="F1369">
+        <v>50</v>
+      </c>
       <c r="H1369">
         <v>50</v>
       </c>
@@ -34121,7 +34763,7 @@
         <v>1</v>
       </c>
       <c r="F1406">
-        <v>42</v>
+        <v>42.09</v>
       </c>
       <c r="H1406">
         <v>42</v>
@@ -35387,6 +36029,9 @@
       <c r="E1461">
         <v>7</v>
       </c>
+      <c r="F1461">
+        <v>980</v>
+      </c>
       <c r="H1461">
         <v>980</v>
       </c>
@@ -35405,6 +36050,9 @@
       <c r="E1462">
         <v>4</v>
       </c>
+      <c r="F1462">
+        <v>240</v>
+      </c>
       <c r="H1462">
         <v>240</v>
       </c>
@@ -35423,6 +36071,9 @@
       <c r="E1463">
         <v>4</v>
       </c>
+      <c r="F1463">
+        <v>360</v>
+      </c>
       <c r="H1463">
         <v>360</v>
       </c>
@@ -35441,6 +36092,9 @@
       <c r="E1464">
         <v>4</v>
       </c>
+      <c r="F1464">
+        <v>100</v>
+      </c>
       <c r="H1464">
         <v>100</v>
       </c>
@@ -35483,6 +36137,9 @@
       <c r="E1466">
         <v>3.5</v>
       </c>
+      <c r="F1466">
+        <v>175</v>
+      </c>
       <c r="H1466">
         <v>175</v>
       </c>
@@ -35501,6 +36158,9 @@
       <c r="E1467">
         <v>1</v>
       </c>
+      <c r="F1467">
+        <v>30</v>
+      </c>
       <c r="H1467">
         <v>30</v>
       </c>
@@ -35519,6 +36179,9 @@
       <c r="E1468">
         <v>2</v>
       </c>
+      <c r="F1468">
+        <v>60</v>
+      </c>
       <c r="H1468">
         <v>60</v>
       </c>
@@ -36936,6 +37599,9 @@
       <c r="E1528">
         <v>1</v>
       </c>
+      <c r="F1528">
+        <v>110</v>
+      </c>
       <c r="H1528">
         <v>110</v>
       </c>
@@ -36957,6 +37623,9 @@
       <c r="E1529">
         <v>1.75</v>
       </c>
+      <c r="F1529">
+        <v>87.5</v>
+      </c>
       <c r="H1529">
         <v>87.5</v>
       </c>
@@ -36978,6 +37647,9 @@
       <c r="E1530">
         <v>1</v>
       </c>
+      <c r="F1530">
+        <v>250</v>
+      </c>
       <c r="H1530">
         <v>250</v>
       </c>
@@ -37992,6 +38664,9 @@
       <c r="E1573">
         <v>2.5</v>
       </c>
+      <c r="F1573">
+        <v>450</v>
+      </c>
       <c r="H1573">
         <v>450</v>
       </c>
@@ -38040,6 +38715,9 @@
       <c r="E1575">
         <v>1</v>
       </c>
+      <c r="F1575">
+        <v>250</v>
+      </c>
       <c r="H1575">
         <v>250</v>
       </c>
@@ -38061,6 +38739,9 @@
       <c r="E1576">
         <v>3</v>
       </c>
+      <c r="F1576">
+        <v>120</v>
+      </c>
       <c r="H1576">
         <v>120</v>
       </c>
@@ -38635,6 +39316,9 @@
       </c>
       <c r="E1600">
         <v>1</v>
+      </c>
+      <c r="F1600">
+        <v>50</v>
       </c>
       <c r="H1600">
         <v>50</v>

</xml_diff>